<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@344717eed51f5b5c8a2aaf2514338156f9ffcbd1 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-medication-adherence.xlsx
+++ b/StructureDefinition-us-core-medication-adherence.xlsx
@@ -84,7 +84,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>A MedicationRequest extension representing reported adherence to prescribed medication instructions.  In other words, whether a medication was consumed according to instructions.</t>
+    <t>The Medication Adherence Extension is a statement of whether a medication has been consumed according to instructions for discharge, community-prescribed, and self-prescribed medications. This extension is not intended to track adherence to the Inpatient Medication Administration Record (MAR). In FHIR, [MedicationAdministration](https://hl7.org/fhir/R4/medicationadministration.html) is typically used to monitor compliance with the MAR.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -294,7 +294,7 @@
     <t>This set of values contains terms representing whether a medication has been consumed according to instructions.</t>
   </si>
   <si>
-    <t>http://cts.nlm.nih.gov/fhir/ValueSet/2.16.840.1.113762.1.4.1099.59</t>
+    <t>http://cts.nlm.nih.gov/fhir/ValueSet/2.16.840.1.113762.1.4.1240.8</t>
   </si>
   <si>
     <t>Extension.value[x]</t>
@@ -720,7 +720,7 @@
     <col min="23" max="23" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="10.53125" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="107.27734375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="63.01953125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="61.8515625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="10.26171875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>

</xml_diff>